<commit_message>
Add diknas course and diknas conversion
</commit_message>
<xml_diff>
--- a/public/uploads/Importgrade.xlsx
+++ b/public/uploads/Importgrade.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="64">
   <si>
     <t>Alexander Ansel Hadipranoto</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Count</t>
   </si>
   <si>
-    <t>12HR-NS</t>
-  </si>
-  <si>
     <t>School Year</t>
   </si>
   <si>
@@ -215,6 +212,12 @@
   </si>
   <si>
     <t>S1Avg</t>
+  </si>
+  <si>
+    <t>Grade 12A</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -584,7 +587,7 @@
   <dimension ref="A1:H726"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E3" sqref="E3:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +596,7 @@
     <col min="2" max="2" width="12.5703125" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="10" bestFit="1" customWidth="1"/>
@@ -605,25 +608,25 @@
         <v>53</v>
       </c>
       <c r="B1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="G1" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -633,21 +636,20 @@
       <c r="B2" s="6">
         <v>20080301</v>
       </c>
-      <c r="C2" s="6" t="str">
-        <f>LEFT(E2,2)</f>
-        <v>12</v>
+      <c r="C2" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F2" s="6">
         <v>82</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="10">
         <v>1</v>
@@ -660,21 +662,20 @@
       <c r="B3" s="6">
         <v>20080301</v>
       </c>
-      <c r="C3" s="6" t="str">
-        <f t="shared" ref="C3:C12" si="0">LEFT(E3,2)</f>
-        <v>12</v>
+      <c r="C3" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F3" s="6">
         <v>76</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H3" s="10">
         <v>1</v>
@@ -687,21 +688,20 @@
       <c r="B4" s="6">
         <v>20080301</v>
       </c>
-      <c r="C4" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C4" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F4" s="6">
         <v>87</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="10">
         <v>1</v>
@@ -714,21 +714,20 @@
       <c r="B5" s="6">
         <v>20080301</v>
       </c>
-      <c r="C5" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C5" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F5" s="6">
         <v>85</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H5" s="10">
         <v>1</v>
@@ -741,21 +740,20 @@
       <c r="B6" s="6">
         <v>20080301</v>
       </c>
-      <c r="C6" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C6" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F6" s="6">
         <v>96</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="10">
         <v>1</v>
@@ -768,21 +766,20 @@
       <c r="B7" s="6">
         <v>20080301</v>
       </c>
-      <c r="C7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C7" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F7" s="6">
         <v>86</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H7" s="10">
         <v>1</v>
@@ -795,21 +792,20 @@
       <c r="B8" s="6">
         <v>20080301</v>
       </c>
-      <c r="C8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C8" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F8" s="6">
         <v>81</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="10">
         <v>1</v>
@@ -822,21 +818,20 @@
       <c r="B9" s="6">
         <v>20080301</v>
       </c>
-      <c r="C9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C9" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F9" s="6">
         <v>80</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H9" s="10">
         <v>1</v>
@@ -849,21 +844,20 @@
       <c r="B10" s="6">
         <v>20080301</v>
       </c>
-      <c r="C10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C10" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F10" s="6">
         <v>95</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H10" s="10">
         <v>1</v>
@@ -876,21 +870,20 @@
       <c r="B11" s="6">
         <v>20080301</v>
       </c>
-      <c r="C11" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C11" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F11" s="6">
         <v>96</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H11" s="10">
         <v>1</v>
@@ -903,21 +896,20 @@
       <c r="B12" s="6">
         <v>20080301</v>
       </c>
-      <c r="C12" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>12</v>
+      <c r="C12" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="F12" s="6">
         <v>92</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H12" s="10">
         <v>1</v>

</xml_diff>